<commit_message>
added lines for notes ... check in print
</commit_message>
<xml_diff>
--- a/diary_a.xlsx
+++ b/diary_a.xlsx
@@ -71,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -230,6 +230,24 @@
       <top style="hair">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
       <bottom style="hair">
         <color indexed="64"/>
       </bottom>
@@ -287,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -309,6 +327,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -598,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,12 +645,12 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
@@ -649,12 +669,12 @@
       <c r="E3" s="9"/>
       <c r="F3" s="15"/>
       <c r="G3" s="9"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -666,13 +686,13 @@
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="18"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -684,12 +704,12 @@
       <c r="E5" s="13"/>
       <c r="F5" s="5"/>
       <c r="G5" s="4"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -701,13 +721,13 @@
       <c r="E6" s="13"/>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="18"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -719,12 +739,12 @@
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -736,13 +756,13 @@
       <c r="E8" s="13"/>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="18"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -765,12 +785,12 @@
       <c r="E10" s="13"/>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -968,6 +988,438 @@
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
     </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>